<commit_message>
correct estimate to make sure that the sign is correct
</commit_message>
<xml_diff>
--- a/ordinal_logistic_sunscreen_stratified_by_race_weight_perception_INDFMPIR_RIDAGEYR.xlsx
+++ b/ordinal_logistic_sunscreen_stratified_by_race_weight_perception_INDFMPIR_RIDAGEYR.xlsx
@@ -368,7 +368,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="n">
-        <v>0.08255214248210986</v>
+        <v>-0.08255214248210986</v>
       </c>
       <c r="E2" t="n">
         <v>0.15335790110779343</v>
@@ -400,7 +400,7 @@
         <v>66</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2839906884612422</v>
+        <v>0.2839906884612422</v>
       </c>
       <c r="E3" t="n">
         <v>0.04555538509949519</v>
@@ -432,7 +432,7 @@
         <v>67</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007775693861353383</v>
+        <v>-0.007775693861353383</v>
       </c>
       <c r="E4" t="n">
         <v>0.006680658061200711</v>
@@ -464,7 +464,7 @@
         <v>68</v>
       </c>
       <c r="D5" t="n">
-        <v>-2.0874616211373374</v>
+        <v>2.0874616211373374</v>
       </c>
       <c r="E5" t="n">
         <v>0.3036925406935181</v>
@@ -496,7 +496,7 @@
         <v>69</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.164123795071367</v>
+        <v>1.164123795071367</v>
       </c>
       <c r="E6" t="n">
         <v>0.2957955155546944</v>
@@ -528,7 +528,7 @@
         <v>70</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.18015132437812764</v>
+        <v>0.18015132437812764</v>
       </c>
       <c r="E7" t="n">
         <v>0.29069760558519736</v>
@@ -560,7 +560,7 @@
         <v>71</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3462003615093696</v>
+        <v>-0.3462003615093696</v>
       </c>
       <c r="E8" t="n">
         <v>0.28960074778616035</v>
@@ -592,7 +592,7 @@
         <v>65</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.056914177885919404</v>
+        <v>0.056914177885919404</v>
       </c>
       <c r="E9" t="n">
         <v>0.08428752549180017</v>
@@ -624,7 +624,7 @@
         <v>66</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.348808453988213</v>
+        <v>0.348808453988213</v>
       </c>
       <c r="E10" t="n">
         <v>0.024614057141759932</v>
@@ -656,7 +656,7 @@
         <v>67</v>
       </c>
       <c r="D11" t="n">
-        <v>0.005404448821220388</v>
+        <v>-0.005404448821220388</v>
       </c>
       <c r="E11" t="n">
         <v>0.003485463539732048</v>
@@ -688,7 +688,7 @@
         <v>68</v>
       </c>
       <c r="D12" t="n">
-        <v>-3.5613800728974114</v>
+        <v>3.5613800728974114</v>
       </c>
       <c r="E12" t="n">
         <v>0.16213166482326027</v>
@@ -720,7 +720,7 @@
         <v>69</v>
       </c>
       <c r="D13" t="n">
-        <v>-2.853528583535301</v>
+        <v>2.853528583535301</v>
       </c>
       <c r="E13" t="n">
         <v>0.15246087941020955</v>
@@ -752,7 +752,7 @@
         <v>70</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.866144724884211</v>
+        <v>1.866144724884211</v>
       </c>
       <c r="E14" t="n">
         <v>0.1453455133338184</v>
@@ -784,7 +784,7 @@
         <v>71</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.2623625533545197</v>
+        <v>1.2623625533545197</v>
       </c>
       <c r="E15" t="n">
         <v>0.14288056063054974</v>
@@ -816,7 +816,7 @@
         <v>65</v>
       </c>
       <c r="D16" t="n">
-        <v>0.23582619410328176</v>
+        <v>-0.23582619410328176</v>
       </c>
       <c r="E16" t="n">
         <v>0.05246276567104126</v>
@@ -848,7 +848,7 @@
         <v>66</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.3010106170290249</v>
+        <v>0.3010106170290249</v>
       </c>
       <c r="E17" t="n">
         <v>0.01513232250879199</v>
@@ -880,7 +880,7 @@
         <v>67</v>
       </c>
       <c r="D18" t="n">
-        <v>0.004002491631060583</v>
+        <v>-0.004002491631060583</v>
       </c>
       <c r="E18" t="n">
         <v>0.0022605869946538894</v>
@@ -912,7 +912,7 @@
         <v>68</v>
       </c>
       <c r="D19" t="n">
-        <v>-2.1284451200434</v>
+        <v>2.1284451200434</v>
       </c>
       <c r="E19" t="n">
         <v>0.09939134745163893</v>
@@ -944,7 +944,7 @@
         <v>69</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.9194854218349113</v>
+        <v>0.9194854218349113</v>
       </c>
       <c r="E20" t="n">
         <v>0.09576124508741796</v>
@@ -976,7 +976,7 @@
         <v>70</v>
       </c>
       <c r="D21" t="n">
-        <v>0.14684595777761356</v>
+        <v>-0.14684595777761356</v>
       </c>
       <c r="E21" t="n">
         <v>0.0950395692427383</v>
@@ -1008,7 +1008,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8889556195355081</v>
+        <v>-0.8889556195355081</v>
       </c>
       <c r="E22" t="n">
         <v>0.09625044589564458</v>
@@ -1040,7 +1040,7 @@
         <v>65</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01989472742147721</v>
+        <v>-0.01989472742147721</v>
       </c>
       <c r="E23" t="n">
         <v>0.08560355272445291</v>
@@ -1072,7 +1072,7 @@
         <v>66</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.29013242509725395</v>
+        <v>0.29013242509725395</v>
       </c>
       <c r="E24" t="n">
         <v>0.027480964205470842</v>
@@ -1104,7 +1104,7 @@
         <v>67</v>
       </c>
       <c r="D25" t="n">
-        <v>0.007208943650491873</v>
+        <v>-0.007208943650491873</v>
       </c>
       <c r="E25" t="n">
         <v>0.003639888559460633</v>
@@ -1136,7 +1136,7 @@
         <v>68</v>
       </c>
       <c r="D26" t="n">
-        <v>-2.0578112888023754</v>
+        <v>2.0578112888023754</v>
       </c>
       <c r="E26" t="n">
         <v>0.15611376054147272</v>
@@ -1168,7 +1168,7 @@
         <v>69</v>
       </c>
       <c r="D27" t="n">
-        <v>-1.3472166621833663</v>
+        <v>1.3472166621833663</v>
       </c>
       <c r="E27" t="n">
         <v>0.15128412422109472</v>
@@ -1200,7 +1200,7 @@
         <v>70</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.391435252170523</v>
+        <v>0.391435252170523</v>
       </c>
       <c r="E28" t="n">
         <v>0.14842962950887756</v>
@@ -1232,7 +1232,7 @@
         <v>71</v>
       </c>
       <c r="D29" t="n">
-        <v>0.170393242966272</v>
+        <v>-0.170393242966272</v>
       </c>
       <c r="E29" t="n">
         <v>0.14851982829400484</v>
@@ -1264,7 +1264,7 @@
         <v>65</v>
       </c>
       <c r="D30" t="n">
-        <v>0.06832384193571298</v>
+        <v>-0.06832384193571298</v>
       </c>
       <c r="E30" t="n">
         <v>0.11614618254126491</v>
@@ -1296,7 +1296,7 @@
         <v>66</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.32115545055127737</v>
+        <v>0.32115545055127737</v>
       </c>
       <c r="E31" t="n">
         <v>0.03627318314109282</v>
@@ -1328,7 +1328,7 @@
         <v>67</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.0147627989462052</v>
+        <v>0.0147627989462052</v>
       </c>
       <c r="E32" t="n">
         <v>0.004919201040519609</v>
@@ -1360,7 +1360,7 @@
         <v>68</v>
       </c>
       <c r="D33" t="n">
-        <v>-2.5056012476238365</v>
+        <v>2.5056012476238365</v>
       </c>
       <c r="E33" t="n">
         <v>0.22286501830304958</v>
@@ -1392,7 +1392,7 @@
         <v>69</v>
       </c>
       <c r="D34" t="n">
-        <v>-1.9228559756444445</v>
+        <v>1.9228559756444445</v>
       </c>
       <c r="E34" t="n">
         <v>0.21746781103436585</v>
@@ -1424,7 +1424,7 @@
         <v>70</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.9379737974650472</v>
+        <v>0.9379737974650472</v>
       </c>
       <c r="E35" t="n">
         <v>0.21089636443009302</v>
@@ -1456,7 +1456,7 @@
         <v>71</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.3555734111623384</v>
+        <v>0.3555734111623384</v>
       </c>
       <c r="E36" t="n">
         <v>0.20963611742534627</v>
@@ -1488,7 +1488,7 @@
         <v>65</v>
       </c>
       <c r="D37" t="n">
-        <v>0.38876659193151175</v>
+        <v>-0.38876659193151175</v>
       </c>
       <c r="E37" t="n">
         <v>0.11701938505907798</v>
@@ -1520,7 +1520,7 @@
         <v>66</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.30037761681707115</v>
+        <v>0.30037761681707115</v>
       </c>
       <c r="E38" t="n">
         <v>0.03595597837599817</v>
@@ -1552,7 +1552,7 @@
         <v>67</v>
       </c>
       <c r="D39" t="n">
-        <v>0.010657592390477585</v>
+        <v>-0.010657592390477585</v>
       </c>
       <c r="E39" t="n">
         <v>0.005457252239656325</v>
@@ -1584,7 +1584,7 @@
         <v>68</v>
       </c>
       <c r="D40" t="n">
-        <v>-1.5306081471471071</v>
+        <v>1.5306081471471071</v>
       </c>
       <c r="E40" t="n">
         <v>0.24966683882645233</v>
@@ -1616,7 +1616,7 @@
         <v>69</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.7659264615090088</v>
+        <v>0.7659264615090088</v>
       </c>
       <c r="E41" t="n">
         <v>0.24525017760578205</v>
@@ -1648,7 +1648,7 @@
         <v>70</v>
       </c>
       <c r="D42" t="n">
-        <v>0.2677207357274053</v>
+        <v>-0.2677207357274053</v>
       </c>
       <c r="E42" t="n">
         <v>0.24348716491502587</v>
@@ -1680,7 +1680,7 @@
         <v>71</v>
       </c>
       <c r="D43" t="n">
-        <v>0.8526298727135938</v>
+        <v>-0.8526298727135938</v>
       </c>
       <c r="E43" t="n">
         <v>0.2457822895464833</v>
@@ -1712,7 +1712,7 @@
         <v>65</v>
       </c>
       <c r="D44" t="n">
-        <v>0.1645829740278381</v>
+        <v>-0.1645829740278381</v>
       </c>
       <c r="E44" t="n">
         <v>0.033414977849147084</v>
@@ -1744,7 +1744,7 @@
         <v>66</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.3413371925493234</v>
+        <v>0.3413371925493234</v>
       </c>
       <c r="E45" t="n">
         <v>0.009840378349628344</v>
@@ -1776,7 +1776,7 @@
         <v>67</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0048468622584794145</v>
+        <v>-0.0048468622584794145</v>
       </c>
       <c r="E46" t="n">
         <v>0.0014459195528606203</v>
@@ -1808,7 +1808,7 @@
         <v>68</v>
       </c>
       <c r="D47" t="n">
-        <v>-2.353484485937728</v>
+        <v>2.353484485937728</v>
       </c>
       <c r="E47" t="n">
         <v>0.0638389696235792</v>
@@ -1840,7 +1840,7 @@
         <v>69</v>
       </c>
       <c r="D48" t="n">
-        <v>-1.4297890791988999</v>
+        <v>1.4297890791988999</v>
       </c>
       <c r="E48" t="n">
         <v>0.06149880372228167</v>
@@ -1872,7 +1872,7 @@
         <v>70</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.487452364232151</v>
+        <v>0.487452364232151</v>
       </c>
       <c r="E49" t="n">
         <v>0.06033567974326661</v>
@@ -1904,7 +1904,7 @@
         <v>71</v>
       </c>
       <c r="D50" t="n">
-        <v>0.083900447581571</v>
+        <v>-0.083900447581571</v>
       </c>
       <c r="E50" t="n">
         <v>0.060221980888525296</v>

</xml_diff>